<commit_message>
Task 2 - Dodano parę aplikacji
</commit_message>
<xml_diff>
--- a/dane_aplikacji.xlsx
+++ b/dane_aplikacji.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zygmunt\Desktop\mgr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="9015"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="551">
   <si>
     <t>Id</t>
   </si>
@@ -1631,17 +1636,71 @@
     <t>klawiatura własna</t>
   </si>
   <si>
-    <t>ilość instalacji</t>
-  </si>
-  <si>
     <t>ocena</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>ilość opini</t>
+  </si>
+  <si>
+    <t>ilosc instalcji</t>
+  </si>
+  <si>
+    <t>50k-100k</t>
+  </si>
+  <si>
+    <t>100k-500k</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>1kk-5kk</t>
+  </si>
+  <si>
+    <t>5k-10k</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>500k-1kk</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>10k-50k</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>5kk-10kk</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>14-11-2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1673,6 +1732,12 @@
       <color theme="1"/>
       <name val="MS Gothic"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1755,7 +1820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1787,19 +1852,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1837,9 +1925,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1871,9 +1959,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1905,9 +1994,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2080,57 +2170,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.140625" style="12" customWidth="1"/>
-    <col min="14" max="19" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="0.85546875" style="12" customWidth="1"/>
-    <col min="21" max="23" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.28515625" style="12" customWidth="1"/>
-    <col min="26" max="27" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="0.7109375" style="12" customWidth="1"/>
-    <col min="33" max="34" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="0.85546875" style="12" customWidth="1"/>
-    <col min="36" max="39" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="1.140625" style="12" customWidth="1"/>
-    <col min="41" max="42" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="1.140625" style="12" customWidth="1"/>
-    <col min="45" max="49" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10.75" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="14.75" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="1.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.125" style="12" customWidth="1"/>
+    <col min="14" max="19" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="0.875" style="12" customWidth="1"/>
+    <col min="21" max="23" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.25" style="12" customWidth="1"/>
+    <col min="26" max="27" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="0.75" style="12" customWidth="1"/>
+    <col min="33" max="34" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="0.875" style="12" customWidth="1"/>
+    <col min="36" max="39" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="1.125" style="12" customWidth="1"/>
+    <col min="41" max="42" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="1.125" style="12" customWidth="1"/>
+    <col min="45" max="49" width="3.875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="1" style="12" customWidth="1"/>
-    <col min="51" max="51" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="3.85546875" customWidth="1"/>
-    <col min="53" max="53" width="1.140625" style="12" customWidth="1"/>
-    <col min="54" max="55" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="0.7109375" style="12" customWidth="1"/>
-    <col min="57" max="58" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="3.875" customWidth="1"/>
+    <col min="53" max="53" width="1.125" style="12" customWidth="1"/>
+    <col min="54" max="55" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="0.75" style="12" customWidth="1"/>
+    <col min="57" max="58" width="3.875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="1" style="12" customWidth="1"/>
-    <col min="60" max="61" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="3.875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="1" style="12" customWidth="1"/>
-    <col min="63" max="64" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="1.140625" style="12" customWidth="1"/>
-    <col min="66" max="69" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="1.125" style="12" customWidth="1"/>
+    <col min="66" max="69" width="3.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="75.75" customHeight="1">
+    <row r="1" spans="1:69" ht="92.25" customHeight="1">
       <c r="H1" t="s">
         <v>482</v>
       </c>
@@ -2235,7 +2325,7 @@
       <c r="BM1" s="10"/>
       <c r="BN1" s="7"/>
     </row>
-    <row r="2" spans="1:69" ht="92.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:69" ht="159.75" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2249,10 +2339,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>532</v>
+      <c r="G2" s="13" t="s">
+        <v>534</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>438</v>
@@ -2416,12 +2509,21 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>550</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4">
+        <v>1327</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -2491,12 +2593,21 @@
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>550</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4">
+        <v>1368</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>535</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -2572,6 +2683,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -2635,18 +2747,19 @@
       <c r="BQ5" s="9"/>
     </row>
     <row r="6" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="4"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -2709,80 +2822,113 @@
       <c r="BP6" s="9"/>
       <c r="BQ6" s="9"/>
     </row>
-    <row r="7" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="E7" s="17">
+        <v>3056</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>536</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11">
+        <v>1</v>
+      </c>
       <c r="M7" s="11"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
+      <c r="N7" s="11">
+        <v>1</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11">
+        <v>1</v>
+      </c>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11">
+        <v>1</v>
+      </c>
       <c r="AI7" s="11"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="11"/>
       <c r="AN7" s="11"/>
-      <c r="AO7" s="9"/>
-      <c r="AP7" s="9"/>
-      <c r="AQ7" s="9"/>
+      <c r="AO7" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="11"/>
+      <c r="AQ7" s="11"/>
       <c r="AR7" s="11"/>
-      <c r="AS7" s="9"/>
-      <c r="AT7" s="9"/>
-      <c r="AU7" s="9"/>
-      <c r="AV7" s="9"/>
-      <c r="AW7" s="9"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="11"/>
+      <c r="AV7" s="11"/>
+      <c r="AW7" s="11">
+        <v>1</v>
+      </c>
       <c r="AX7" s="11"/>
-      <c r="AY7" s="9"/>
-      <c r="AZ7" s="9"/>
+      <c r="AY7" s="11"/>
+      <c r="AZ7" s="11">
+        <v>1</v>
+      </c>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="9"/>
-      <c r="BC7" s="9"/>
+      <c r="BB7" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC7" s="11"/>
       <c r="BD7" s="11"/>
-      <c r="BE7" s="9"/>
-      <c r="BF7" s="9"/>
+      <c r="BE7" s="11"/>
+      <c r="BF7" s="11">
+        <v>1</v>
+      </c>
       <c r="BG7" s="11"/>
-      <c r="BH7" s="9"/>
-      <c r="BI7" s="9"/>
+      <c r="BH7" s="11"/>
+      <c r="BI7" s="11">
+        <v>1</v>
+      </c>
       <c r="BJ7" s="11"/>
-      <c r="BK7" s="9"/>
-      <c r="BL7" s="9"/>
+      <c r="BK7" s="11"/>
+      <c r="BL7" s="11"/>
       <c r="BM7" s="11"/>
-      <c r="BN7" s="9"/>
-      <c r="BO7" s="9"/>
-      <c r="BP7" s="9"/>
-      <c r="BQ7" s="9"/>
+      <c r="BN7" s="11"/>
+      <c r="BO7" s="11"/>
+      <c r="BP7" s="11"/>
+      <c r="BQ7" s="11"/>
     </row>
     <row r="8" spans="1:69" ht="16.5" thickBot="1">
       <c r="A8" s="3" t="s">
@@ -2791,12 +2937,21 @@
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>550</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4">
+        <v>5310</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -2859,19 +3014,28 @@
       <c r="BP8" s="9"/>
       <c r="BQ8" s="9"/>
     </row>
-    <row r="9" spans="1:69" ht="16.5" thickBot="1">
+    <row r="9" spans="1:69" ht="17.25" customHeight="1" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>550</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="4">
+        <v>3884</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -2934,380 +3098,575 @@
       <c r="BP9" s="9"/>
       <c r="BQ9" s="9"/>
     </row>
-    <row r="10" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:69" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="E10" s="17">
+        <v>16461</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="I10" s="11">
+        <v>1</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
       <c r="M10" s="11"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11">
+        <v>1</v>
+      </c>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11">
+        <v>1</v>
+      </c>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11">
+        <v>1</v>
+      </c>
       <c r="AI10" s="11"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="9"/>
+      <c r="AJ10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
       <c r="AN10" s="11"/>
-      <c r="AO10" s="9"/>
-      <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
       <c r="AR10" s="11"/>
-      <c r="AS10" s="9"/>
-      <c r="AT10" s="9"/>
-      <c r="AU10" s="9"/>
-      <c r="AV10" s="9"/>
-      <c r="AW10" s="9"/>
+      <c r="AS10" s="11"/>
+      <c r="AT10" s="11"/>
+      <c r="AU10" s="11"/>
+      <c r="AV10" s="11"/>
+      <c r="AW10" s="11">
+        <v>1</v>
+      </c>
       <c r="AX10" s="11"/>
-      <c r="AY10" s="9"/>
-      <c r="AZ10" s="9"/>
+      <c r="AY10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ10" s="11"/>
       <c r="BA10" s="11"/>
-      <c r="BB10" s="9"/>
-      <c r="BC10" s="9"/>
+      <c r="BB10" s="11"/>
+      <c r="BC10" s="11">
+        <v>1</v>
+      </c>
       <c r="BD10" s="11"/>
-      <c r="BE10" s="9"/>
-      <c r="BF10" s="9"/>
+      <c r="BE10" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF10" s="11"/>
       <c r="BG10" s="11"/>
-      <c r="BH10" s="9"/>
-      <c r="BI10" s="9"/>
+      <c r="BH10" s="11"/>
+      <c r="BI10" s="11">
+        <v>1</v>
+      </c>
       <c r="BJ10" s="11"/>
-      <c r="BK10" s="9"/>
-      <c r="BL10" s="9"/>
+      <c r="BK10" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL10" s="11">
+        <v>1</v>
+      </c>
       <c r="BM10" s="11"/>
-      <c r="BN10" s="9"/>
-      <c r="BO10" s="9"/>
-      <c r="BP10" s="9"/>
-      <c r="BQ10" s="9"/>
-    </row>
-    <row r="11" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A11" s="3" t="s">
+      <c r="BN10" s="11">
+        <v>1</v>
+      </c>
+      <c r="BO10" s="11"/>
+      <c r="BP10" s="11"/>
+      <c r="BQ10" s="11"/>
+    </row>
+    <row r="11" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="E11" s="17">
+        <v>72</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
+      <c r="Z11" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11">
+        <v>1</v>
+      </c>
       <c r="AI11" s="11"/>
-      <c r="AJ11" s="9"/>
-      <c r="AK11" s="9"/>
-      <c r="AL11" s="9"/>
-      <c r="AM11" s="9"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
       <c r="AN11" s="11"/>
-      <c r="AO11" s="9"/>
-      <c r="AP11" s="9"/>
-      <c r="AQ11" s="9"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
+      <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
-      <c r="AS11" s="9"/>
-      <c r="AT11" s="9"/>
-      <c r="AU11" s="9"/>
-      <c r="AV11" s="9"/>
-      <c r="AW11" s="9"/>
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11"/>
+      <c r="AV11" s="11"/>
+      <c r="AW11" s="11">
+        <v>1</v>
+      </c>
       <c r="AX11" s="11"/>
-      <c r="AY11" s="9"/>
-      <c r="AZ11" s="9"/>
+      <c r="AY11" s="11"/>
+      <c r="AZ11" s="11">
+        <v>1</v>
+      </c>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="9"/>
-      <c r="BC11" s="9"/>
+      <c r="BB11" s="11"/>
+      <c r="BC11" s="11">
+        <v>1</v>
+      </c>
       <c r="BD11" s="11"/>
-      <c r="BE11" s="9"/>
-      <c r="BF11" s="9"/>
+      <c r="BE11" s="11"/>
+      <c r="BF11" s="11">
+        <v>1</v>
+      </c>
       <c r="BG11" s="11"/>
-      <c r="BH11" s="9"/>
-      <c r="BI11" s="9"/>
+      <c r="BH11" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI11" s="11"/>
       <c r="BJ11" s="11"/>
-      <c r="BK11" s="9"/>
-      <c r="BL11" s="9"/>
+      <c r="BK11" s="11"/>
+      <c r="BL11" s="11"/>
       <c r="BM11" s="11"/>
-      <c r="BN11" s="9"/>
-      <c r="BO11" s="9"/>
-      <c r="BP11" s="9"/>
-      <c r="BQ11" s="9"/>
-    </row>
-    <row r="12" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A12" s="3" t="s">
+      <c r="BN11" s="11"/>
+      <c r="BO11" s="11"/>
+      <c r="BP11" s="11"/>
+      <c r="BQ11" s="11"/>
+    </row>
+    <row r="12" spans="1:69" s="12" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="E12" s="17">
+        <v>18392</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>542</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>543</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11">
+        <v>1</v>
+      </c>
       <c r="M12" s="11"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
+      <c r="N12" s="11">
+        <v>1</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11">
+        <v>1</v>
+      </c>
       <c r="T12" s="11"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11">
+        <v>1</v>
+      </c>
       <c r="Y12" s="11"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
+      <c r="Z12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11">
+        <v>1</v>
+      </c>
       <c r="AI12" s="11"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
-      <c r="AL12" s="9"/>
-      <c r="AM12" s="9"/>
+      <c r="AJ12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="11"/>
       <c r="AN12" s="11"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11"/>
+      <c r="AQ12" s="11"/>
       <c r="AR12" s="11"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
-      <c r="AW12" s="9"/>
+      <c r="AS12" s="11"/>
+      <c r="AT12" s="11"/>
+      <c r="AU12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="11"/>
+      <c r="AW12" s="11"/>
       <c r="AX12" s="11"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
+      <c r="AY12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ12" s="11"/>
       <c r="BA12" s="11"/>
-      <c r="BB12" s="9"/>
-      <c r="BC12" s="9"/>
+      <c r="BB12" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="11"/>
       <c r="BD12" s="11"/>
-      <c r="BE12" s="9"/>
-      <c r="BF12" s="9"/>
+      <c r="BE12" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF12" s="11"/>
       <c r="BG12" s="11"/>
-      <c r="BH12" s="9"/>
-      <c r="BI12" s="9"/>
+      <c r="BH12" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI12" s="11"/>
       <c r="BJ12" s="11"/>
-      <c r="BK12" s="9"/>
-      <c r="BL12" s="9"/>
+      <c r="BK12" s="11"/>
+      <c r="BL12" s="11"/>
       <c r="BM12" s="11"/>
-      <c r="BN12" s="9"/>
-      <c r="BO12" s="9"/>
-      <c r="BP12" s="9"/>
-      <c r="BQ12" s="9"/>
-    </row>
-    <row r="13" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A13" s="3" t="s">
+      <c r="BN12" s="11"/>
+      <c r="BO12" s="11"/>
+      <c r="BP12" s="11"/>
+      <c r="BQ12" s="11"/>
+    </row>
+    <row r="13" spans="1:69" s="12" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="E13" s="17">
+        <v>7895</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>543</v>
+      </c>
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11">
+        <v>1</v>
+      </c>
       <c r="M13" s="11"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11">
+        <v>1</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
       <c r="T13" s="11"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11">
+        <v>1</v>
+      </c>
       <c r="Y13" s="11"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
+      <c r="Z13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11">
+        <v>1</v>
+      </c>
       <c r="AF13" s="11"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11">
+        <v>1</v>
+      </c>
       <c r="AI13" s="11"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
-      <c r="AL13" s="9"/>
-      <c r="AM13" s="9"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="11"/>
       <c r="AN13" s="11"/>
-      <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
-      <c r="AQ13" s="9"/>
+      <c r="AO13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="11"/>
+      <c r="AQ13" s="11"/>
       <c r="AR13" s="11"/>
-      <c r="AS13" s="9"/>
-      <c r="AT13" s="9"/>
-      <c r="AU13" s="9"/>
-      <c r="AV13" s="9"/>
-      <c r="AW13" s="9"/>
+      <c r="AS13" s="11"/>
+      <c r="AT13" s="11"/>
+      <c r="AU13" s="11"/>
+      <c r="AV13" s="11"/>
+      <c r="AW13" s="11">
+        <v>1</v>
+      </c>
       <c r="AX13" s="11"/>
-      <c r="AY13" s="9"/>
-      <c r="AZ13" s="9"/>
+      <c r="AY13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ13" s="11"/>
       <c r="BA13" s="11"/>
-      <c r="BB13" s="9"/>
-      <c r="BC13" s="9"/>
+      <c r="BB13" s="11"/>
+      <c r="BC13" s="11">
+        <v>1</v>
+      </c>
       <c r="BD13" s="11"/>
-      <c r="BE13" s="9"/>
-      <c r="BF13" s="9"/>
+      <c r="BE13" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF13" s="11"/>
       <c r="BG13" s="11"/>
-      <c r="BH13" s="9"/>
-      <c r="BI13" s="9"/>
+      <c r="BH13" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI13" s="11"/>
       <c r="BJ13" s="11"/>
-      <c r="BK13" s="9"/>
-      <c r="BL13" s="9"/>
+      <c r="BK13" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL13" s="11"/>
       <c r="BM13" s="11"/>
-      <c r="BN13" s="9"/>
-      <c r="BO13" s="9"/>
-      <c r="BP13" s="9"/>
-      <c r="BQ13" s="9"/>
-    </row>
-    <row r="14" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A14" s="3" t="s">
+      <c r="BN13" s="11"/>
+      <c r="BO13" s="11"/>
+      <c r="BP13" s="11"/>
+      <c r="BQ13" s="11"/>
+    </row>
+    <row r="14" spans="1:69" s="12" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="E14" s="17">
+        <v>430</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
       <c r="M14" s="11"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11">
+        <v>1</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
       <c r="T14" s="11"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11">
+        <v>1</v>
+      </c>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
+      <c r="Z14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11">
+        <v>1</v>
+      </c>
       <c r="AI14" s="11"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AL14" s="9"/>
-      <c r="AM14" s="9"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="11"/>
       <c r="AN14" s="11"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
+      <c r="AO14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="11"/>
+      <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
-      <c r="AS14" s="9"/>
-      <c r="AT14" s="9"/>
-      <c r="AU14" s="9"/>
-      <c r="AV14" s="9"/>
-      <c r="AW14" s="9"/>
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="11"/>
+      <c r="AU14" s="11"/>
+      <c r="AV14" s="11"/>
+      <c r="AW14" s="11">
+        <v>1</v>
+      </c>
       <c r="AX14" s="11"/>
-      <c r="AY14" s="9"/>
-      <c r="AZ14" s="9"/>
+      <c r="AY14" s="11"/>
+      <c r="AZ14" s="11">
+        <v>1</v>
+      </c>
       <c r="BA14" s="11"/>
-      <c r="BB14" s="9"/>
-      <c r="BC14" s="9"/>
+      <c r="BB14" s="11"/>
+      <c r="BC14" s="11">
+        <v>1</v>
+      </c>
       <c r="BD14" s="11"/>
-      <c r="BE14" s="9"/>
-      <c r="BF14" s="9"/>
+      <c r="BE14" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF14" s="11"/>
       <c r="BG14" s="11"/>
-      <c r="BH14" s="9"/>
-      <c r="BI14" s="9"/>
+      <c r="BH14" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI14" s="11"/>
       <c r="BJ14" s="11"/>
-      <c r="BK14" s="9"/>
-      <c r="BL14" s="9"/>
+      <c r="BK14" s="11"/>
+      <c r="BL14" s="11"/>
       <c r="BM14" s="11"/>
-      <c r="BN14" s="9"/>
-      <c r="BO14" s="9"/>
-      <c r="BP14" s="9"/>
-      <c r="BQ14" s="9"/>
+      <c r="BN14" s="11"/>
+      <c r="BO14" s="11"/>
+      <c r="BP14" s="11"/>
+      <c r="BQ14" s="11"/>
     </row>
     <row r="15" spans="1:69" ht="16.5" thickBot="1">
       <c r="A15" s="3" t="s">
@@ -3322,6 +3681,7 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -3384,605 +3744,909 @@
       <c r="BP15" s="9"/>
       <c r="BQ15" s="9"/>
     </row>
-    <row r="16" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="E16" s="17">
+        <v>314</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
       <c r="M16" s="11"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11">
+        <v>1</v>
+      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
       <c r="T16" s="11"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11">
+        <v>1</v>
+      </c>
+      <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
+      <c r="Z16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
       <c r="AF16" s="11"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
+      <c r="AG16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="11"/>
       <c r="AI16" s="11"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
-      <c r="AL16" s="9"/>
-      <c r="AM16" s="9"/>
+      <c r="AJ16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
       <c r="AN16" s="11"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
+      <c r="AQ16" s="11"/>
       <c r="AR16" s="11"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AU16" s="9"/>
-      <c r="AV16" s="9"/>
-      <c r="AW16" s="9"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="11"/>
+      <c r="AU16" s="11"/>
+      <c r="AV16" s="11"/>
+      <c r="AW16" s="11">
+        <v>1</v>
+      </c>
       <c r="AX16" s="11"/>
-      <c r="AY16" s="9"/>
-      <c r="AZ16" s="9"/>
+      <c r="AY16" s="11"/>
+      <c r="AZ16" s="11">
+        <v>1</v>
+      </c>
       <c r="BA16" s="11"/>
-      <c r="BB16" s="9"/>
-      <c r="BC16" s="9"/>
+      <c r="BB16" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC16" s="11"/>
       <c r="BD16" s="11"/>
-      <c r="BE16" s="9"/>
-      <c r="BF16" s="9"/>
+      <c r="BE16" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF16" s="11"/>
       <c r="BG16" s="11"/>
-      <c r="BH16" s="9"/>
-      <c r="BI16" s="9"/>
+      <c r="BH16" s="11"/>
+      <c r="BI16" s="11">
+        <v>1</v>
+      </c>
       <c r="BJ16" s="11"/>
-      <c r="BK16" s="9"/>
-      <c r="BL16" s="9"/>
+      <c r="BK16" s="11"/>
+      <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
-      <c r="BN16" s="9"/>
-      <c r="BO16" s="9"/>
-      <c r="BP16" s="9"/>
-      <c r="BQ16" s="9"/>
-    </row>
-    <row r="17" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A17" s="3" t="s">
+      <c r="BN16" s="11"/>
+      <c r="BO16" s="11"/>
+      <c r="BP16" s="11"/>
+      <c r="BQ16" s="11"/>
+    </row>
+    <row r="17" spans="1:69" s="12" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
+      <c r="A17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="E17" s="17">
+        <v>1168</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11">
+        <v>1</v>
+      </c>
       <c r="M17" s="11"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11">
+        <v>1</v>
+      </c>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
       <c r="T17" s="11"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11">
+        <v>1</v>
+      </c>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11">
+        <v>1</v>
+      </c>
       <c r="Y17" s="11"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
+      <c r="Z17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
       <c r="AF17" s="11"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11">
+        <v>1</v>
+      </c>
       <c r="AI17" s="11"/>
-      <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
-      <c r="AL17" s="9"/>
-      <c r="AM17" s="9"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="11"/>
+      <c r="AM17" s="11"/>
       <c r="AN17" s="11"/>
-      <c r="AO17" s="9"/>
-      <c r="AP17" s="9"/>
-      <c r="AQ17" s="9"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
+      <c r="AQ17" s="11"/>
       <c r="AR17" s="11"/>
-      <c r="AS17" s="9"/>
-      <c r="AT17" s="9"/>
-      <c r="AU17" s="9"/>
-      <c r="AV17" s="9"/>
-      <c r="AW17" s="9"/>
+      <c r="AS17" s="11"/>
+      <c r="AT17" s="11"/>
+      <c r="AU17" s="11"/>
+      <c r="AV17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="11">
+        <v>1</v>
+      </c>
       <c r="AX17" s="11"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="9"/>
+      <c r="AY17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ17" s="11"/>
       <c r="BA17" s="11"/>
-      <c r="BB17" s="9"/>
-      <c r="BC17" s="9"/>
+      <c r="BB17" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC17" s="11"/>
       <c r="BD17" s="11"/>
-      <c r="BE17" s="9"/>
-      <c r="BF17" s="9"/>
+      <c r="BE17" s="11"/>
+      <c r="BF17" s="11"/>
       <c r="BG17" s="11"/>
-      <c r="BH17" s="9"/>
-      <c r="BI17" s="9"/>
+      <c r="BH17" s="11"/>
+      <c r="BI17" s="11"/>
       <c r="BJ17" s="11"/>
-      <c r="BK17" s="9"/>
-      <c r="BL17" s="9"/>
+      <c r="BK17" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL17" s="11"/>
       <c r="BM17" s="11"/>
-      <c r="BN17" s="9"/>
-      <c r="BO17" s="9"/>
-      <c r="BP17" s="9"/>
-      <c r="BQ17" s="9"/>
-    </row>
-    <row r="18" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A18" s="3" t="s">
+      <c r="BN17" s="11"/>
+      <c r="BO17" s="11"/>
+      <c r="BP17" s="11"/>
+      <c r="BQ17" s="11"/>
+    </row>
+    <row r="18" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" customHeight="1" thickBot="1">
+      <c r="A18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="E18" s="17">
+        <v>64564</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11">
+        <v>1</v>
+      </c>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
       <c r="T18" s="11"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11">
+        <v>1</v>
+      </c>
+      <c r="X18" s="11"/>
       <c r="Y18" s="11"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
       <c r="AF18" s="11"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11">
+        <v>1</v>
+      </c>
       <c r="AI18" s="11"/>
-      <c r="AJ18" s="9"/>
-      <c r="AK18" s="9"/>
-      <c r="AL18" s="9"/>
-      <c r="AM18" s="9"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
       <c r="AN18" s="11"/>
-      <c r="AO18" s="9"/>
-      <c r="AP18" s="9"/>
-      <c r="AQ18" s="9"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
+      <c r="AQ18" s="11"/>
       <c r="AR18" s="11"/>
-      <c r="AS18" s="9"/>
-      <c r="AT18" s="9"/>
-      <c r="AU18" s="9"/>
-      <c r="AV18" s="9"/>
-      <c r="AW18" s="9"/>
+      <c r="AS18" s="11"/>
+      <c r="AT18" s="11"/>
+      <c r="AU18" s="11"/>
+      <c r="AV18" s="11"/>
+      <c r="AW18" s="11">
+        <v>1</v>
+      </c>
       <c r="AX18" s="11"/>
-      <c r="AY18" s="9"/>
-      <c r="AZ18" s="9"/>
+      <c r="AY18" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ18" s="11"/>
       <c r="BA18" s="11"/>
-      <c r="BB18" s="9"/>
-      <c r="BC18" s="9"/>
+      <c r="BB18" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="11"/>
       <c r="BD18" s="11"/>
-      <c r="BE18" s="9"/>
-      <c r="BF18" s="9"/>
+      <c r="BE18" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF18" s="11"/>
       <c r="BG18" s="11"/>
-      <c r="BH18" s="9"/>
-      <c r="BI18" s="9"/>
+      <c r="BH18" s="11"/>
+      <c r="BI18" s="11">
+        <v>1</v>
+      </c>
       <c r="BJ18" s="11"/>
-      <c r="BK18" s="9"/>
-      <c r="BL18" s="9"/>
+      <c r="BK18" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL18" s="11"/>
       <c r="BM18" s="11"/>
-      <c r="BN18" s="9"/>
-      <c r="BO18" s="9"/>
-      <c r="BP18" s="9"/>
-      <c r="BQ18" s="9"/>
-    </row>
-    <row r="19" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A19" s="3" t="s">
+      <c r="BN18" s="11"/>
+      <c r="BO18" s="11"/>
+      <c r="BP18" s="11"/>
+      <c r="BQ18" s="11"/>
+    </row>
+    <row r="19" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="E19" s="17">
+        <v>1217</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>546</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11">
+        <v>1</v>
+      </c>
       <c r="M19" s="11"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11">
+        <v>1</v>
+      </c>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
       <c r="T19" s="11"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
+      <c r="U19" s="11">
+        <v>1</v>
+      </c>
+      <c r="V19" s="11">
+        <v>1</v>
+      </c>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11">
+        <v>1</v>
+      </c>
       <c r="Y19" s="11"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
+      <c r="Z19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="11"/>
       <c r="AF19" s="11"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11">
+        <v>1</v>
+      </c>
       <c r="AI19" s="11"/>
-      <c r="AJ19" s="9"/>
-      <c r="AK19" s="9"/>
-      <c r="AL19" s="9"/>
-      <c r="AM19" s="9"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="11"/>
       <c r="AN19" s="11"/>
-      <c r="AO19" s="9"/>
-      <c r="AP19" s="9"/>
-      <c r="AQ19" s="9"/>
+      <c r="AO19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="11"/>
       <c r="AR19" s="11"/>
-      <c r="AS19" s="9"/>
-      <c r="AT19" s="9"/>
-      <c r="AU19" s="9"/>
-      <c r="AV19" s="9"/>
-      <c r="AW19" s="9"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="11"/>
+      <c r="AV19" s="11"/>
+      <c r="AW19" s="11">
+        <v>1</v>
+      </c>
       <c r="AX19" s="11"/>
-      <c r="AY19" s="9"/>
-      <c r="AZ19" s="9"/>
+      <c r="AY19" s="11"/>
+      <c r="AZ19" s="11">
+        <v>1</v>
+      </c>
       <c r="BA19" s="11"/>
-      <c r="BB19" s="9"/>
-      <c r="BC19" s="9"/>
+      <c r="BB19" s="11"/>
+      <c r="BC19" s="11">
+        <v>1</v>
+      </c>
       <c r="BD19" s="11"/>
-      <c r="BE19" s="9"/>
-      <c r="BF19" s="9"/>
+      <c r="BE19" s="11"/>
+      <c r="BF19" s="11">
+        <v>1</v>
+      </c>
       <c r="BG19" s="11"/>
-      <c r="BH19" s="9"/>
-      <c r="BI19" s="9"/>
+      <c r="BH19" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI19" s="11"/>
       <c r="BJ19" s="11"/>
-      <c r="BK19" s="9"/>
-      <c r="BL19" s="9"/>
+      <c r="BK19" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL19" s="11"/>
       <c r="BM19" s="11"/>
-      <c r="BN19" s="9"/>
-      <c r="BO19" s="9"/>
-      <c r="BP19" s="9"/>
-      <c r="BQ19" s="9"/>
-    </row>
-    <row r="20" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A20" s="3" t="s">
+      <c r="BN19" s="11"/>
+      <c r="BO19" s="11"/>
+      <c r="BP19" s="11"/>
+      <c r="BQ19" s="11"/>
+    </row>
+    <row r="20" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="E20" s="17">
+        <v>336</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11">
+        <v>1</v>
+      </c>
       <c r="M20" s="11"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11">
+        <v>1</v>
+      </c>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
       <c r="T20" s="11"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
+      <c r="U20" s="11">
+        <v>1</v>
+      </c>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
       <c r="AF20" s="11"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="11">
+        <v>1</v>
+      </c>
       <c r="AI20" s="11"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="9"/>
-      <c r="AM20" s="9"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="11"/>
       <c r="AN20" s="11"/>
-      <c r="AO20" s="9"/>
-      <c r="AP20" s="9"/>
-      <c r="AQ20" s="9"/>
+      <c r="AO20" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="11"/>
+      <c r="AQ20" s="11"/>
       <c r="AR20" s="11"/>
-      <c r="AS20" s="9"/>
-      <c r="AT20" s="9"/>
-      <c r="AU20" s="9"/>
-      <c r="AV20" s="9"/>
-      <c r="AW20" s="9"/>
+      <c r="AS20" s="11"/>
+      <c r="AT20" s="11"/>
+      <c r="AU20" s="11"/>
+      <c r="AV20" s="11"/>
+      <c r="AW20" s="11">
+        <v>1</v>
+      </c>
       <c r="AX20" s="11"/>
-      <c r="AY20" s="9"/>
-      <c r="AZ20" s="9"/>
+      <c r="AY20" s="11"/>
+      <c r="AZ20" s="11">
+        <v>1</v>
+      </c>
       <c r="BA20" s="11"/>
-      <c r="BB20" s="9"/>
-      <c r="BC20" s="9"/>
+      <c r="BB20" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="11"/>
       <c r="BD20" s="11"/>
-      <c r="BE20" s="9"/>
-      <c r="BF20" s="9"/>
+      <c r="BE20" s="11"/>
+      <c r="BF20" s="11">
+        <v>1</v>
+      </c>
       <c r="BG20" s="11"/>
-      <c r="BH20" s="9"/>
-      <c r="BI20" s="9"/>
+      <c r="BH20" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI20" s="11"/>
       <c r="BJ20" s="11"/>
-      <c r="BK20" s="9"/>
-      <c r="BL20" s="9"/>
+      <c r="BK20" s="11"/>
+      <c r="BL20" s="11">
+        <v>1</v>
+      </c>
       <c r="BM20" s="11"/>
-      <c r="BN20" s="9"/>
-      <c r="BO20" s="9"/>
-      <c r="BP20" s="9"/>
-      <c r="BQ20" s="9"/>
-    </row>
-    <row r="21" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A21" s="3" t="s">
+      <c r="BN20" s="11">
+        <v>1</v>
+      </c>
+      <c r="BO20" s="11"/>
+      <c r="BP20" s="11"/>
+      <c r="BQ20" s="11"/>
+    </row>
+    <row r="21" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="E21" s="17">
+        <v>82937</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="11"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11">
+        <v>1</v>
+      </c>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
       <c r="T21" s="11"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11">
+        <v>1</v>
+      </c>
       <c r="Y21" s="11"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
+      <c r="Z21" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="11">
+        <v>1</v>
+      </c>
       <c r="AF21" s="11"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
+      <c r="AG21" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="11"/>
       <c r="AI21" s="11"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
+      <c r="AJ21" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
       <c r="AN21" s="11"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AQ21" s="9"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="11"/>
       <c r="AR21" s="11"/>
-      <c r="AS21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="11"/>
+      <c r="AU21" s="11"/>
+      <c r="AV21" s="11"/>
+      <c r="AW21" s="11">
+        <v>1</v>
+      </c>
       <c r="AX21" s="11"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="9"/>
+      <c r="AY21" s="11"/>
+      <c r="AZ21" s="11">
+        <v>1</v>
+      </c>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="9"/>
-      <c r="BC21" s="9"/>
+      <c r="BB21" s="11"/>
+      <c r="BC21" s="11">
+        <v>1</v>
+      </c>
       <c r="BD21" s="11"/>
-      <c r="BE21" s="9"/>
-      <c r="BF21" s="9"/>
+      <c r="BE21" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF21" s="11"/>
       <c r="BG21" s="11"/>
-      <c r="BH21" s="9"/>
-      <c r="BI21" s="9"/>
+      <c r="BH21" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI21" s="11"/>
       <c r="BJ21" s="11"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
+      <c r="BK21" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL21" s="11"/>
       <c r="BM21" s="11"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-    </row>
-    <row r="22" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A22" s="3" t="s">
+      <c r="BN21" s="11"/>
+      <c r="BO21" s="11"/>
+      <c r="BP21" s="11"/>
+      <c r="BQ21" s="11"/>
+    </row>
+    <row r="22" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A22" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="E22" s="17">
+        <v>1788</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>536</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11">
+        <v>1</v>
+      </c>
       <c r="M22" s="11"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11">
+        <v>1</v>
+      </c>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
       <c r="T22" s="11"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11">
+        <v>1</v>
+      </c>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
       <c r="Y22" s="11"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
+      <c r="Z22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="11"/>
       <c r="AF22" s="11"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11">
+        <v>1</v>
+      </c>
       <c r="AI22" s="11"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
-      <c r="AL22" s="9"/>
-      <c r="AM22" s="9"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="11"/>
       <c r="AN22" s="11"/>
-      <c r="AO22" s="9"/>
-      <c r="AP22" s="9"/>
-      <c r="AQ22" s="9"/>
+      <c r="AO22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="11"/>
       <c r="AR22" s="11"/>
-      <c r="AS22" s="9"/>
-      <c r="AT22" s="9"/>
-      <c r="AU22" s="9"/>
-      <c r="AV22" s="9"/>
-      <c r="AW22" s="9"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="11"/>
+      <c r="AU22" s="11"/>
+      <c r="AV22" s="11"/>
+      <c r="AW22" s="11">
+        <v>1</v>
+      </c>
       <c r="AX22" s="11"/>
-      <c r="AY22" s="9"/>
-      <c r="AZ22" s="9"/>
+      <c r="AY22" s="11"/>
+      <c r="AZ22" s="11">
+        <v>1</v>
+      </c>
       <c r="BA22" s="11"/>
-      <c r="BB22" s="9"/>
-      <c r="BC22" s="9"/>
+      <c r="BB22" s="11"/>
+      <c r="BC22" s="11">
+        <v>1</v>
+      </c>
       <c r="BD22" s="11"/>
-      <c r="BE22" s="9"/>
-      <c r="BF22" s="9"/>
+      <c r="BE22" s="11"/>
+      <c r="BF22" s="11">
+        <v>1</v>
+      </c>
       <c r="BG22" s="11"/>
-      <c r="BH22" s="9"/>
-      <c r="BI22" s="9"/>
+      <c r="BH22" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI22" s="11"/>
       <c r="BJ22" s="11"/>
-      <c r="BK22" s="9"/>
-      <c r="BL22" s="9"/>
+      <c r="BK22" s="11"/>
+      <c r="BL22" s="11">
+        <v>1</v>
+      </c>
       <c r="BM22" s="11"/>
-      <c r="BN22" s="9"/>
-      <c r="BO22" s="9"/>
-      <c r="BP22" s="9"/>
-      <c r="BQ22" s="9"/>
-    </row>
-    <row r="23" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A23" s="3" t="s">
+      <c r="BN22" s="11"/>
+      <c r="BO22" s="11"/>
+      <c r="BP22" s="11"/>
+      <c r="BQ22" s="11"/>
+    </row>
+    <row r="23" spans="1:69" s="12" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+      <c r="A23" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="E23" s="17">
+        <v>89317</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>549</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="I23" s="11">
+        <v>1</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11">
+        <v>1</v>
+      </c>
       <c r="M23" s="11"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
+      <c r="N23" s="11">
+        <v>1</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11">
+        <v>1</v>
+      </c>
+      <c r="R23" s="11">
+        <v>1</v>
+      </c>
+      <c r="S23" s="11">
+        <v>1</v>
+      </c>
       <c r="T23" s="11"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
+      <c r="U23" s="11">
+        <v>1</v>
+      </c>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11">
+        <v>1</v>
+      </c>
       <c r="Y23" s="11"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
       <c r="AF23" s="11"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11">
+        <v>1</v>
+      </c>
       <c r="AI23" s="11"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
+      <c r="AJ23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="11"/>
+      <c r="AM23" s="11"/>
       <c r="AN23" s="11"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
-      <c r="AQ23" s="9"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
       <c r="AR23" s="11"/>
-      <c r="AS23" s="9"/>
-      <c r="AT23" s="9"/>
-      <c r="AU23" s="9"/>
-      <c r="AV23" s="9"/>
-      <c r="AW23" s="9"/>
+      <c r="AS23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="11"/>
+      <c r="AV23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AW23" s="11"/>
       <c r="AX23" s="11"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="9"/>
+      <c r="AY23" s="11"/>
+      <c r="AZ23" s="11">
+        <v>1</v>
+      </c>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="9"/>
-      <c r="BC23" s="9"/>
+      <c r="BB23" s="11"/>
+      <c r="BC23" s="11">
+        <v>1</v>
+      </c>
       <c r="BD23" s="11"/>
-      <c r="BE23" s="9"/>
-      <c r="BF23" s="9"/>
+      <c r="BE23" s="11">
+        <v>1</v>
+      </c>
+      <c r="BF23" s="11"/>
       <c r="BG23" s="11"/>
-      <c r="BH23" s="9"/>
-      <c r="BI23" s="9"/>
+      <c r="BH23" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI23" s="11"/>
       <c r="BJ23" s="11"/>
-      <c r="BK23" s="9"/>
-      <c r="BL23" s="9"/>
+      <c r="BK23" s="11">
+        <v>1</v>
+      </c>
+      <c r="BL23" s="11"/>
       <c r="BM23" s="11"/>
-      <c r="BN23" s="9"/>
-      <c r="BO23" s="9"/>
-      <c r="BP23" s="9"/>
-      <c r="BQ23" s="9"/>
+      <c r="BN23" s="11"/>
+      <c r="BO23" s="11"/>
+      <c r="BP23" s="11"/>
+      <c r="BQ23" s="11"/>
     </row>
     <row r="24" spans="1:69" ht="16.5" thickBot="1">
       <c r="A24" s="3" t="s">
@@ -3997,6 +4661,7 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -4072,6 +4737,7 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -4147,6 +4813,7 @@
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -4222,6 +4889,7 @@
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -4297,6 +4965,7 @@
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -4372,6 +5041,7 @@
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -4447,6 +5117,7 @@
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -4522,6 +5193,7 @@
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -4597,6 +5269,7 @@
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -4672,6 +5345,7 @@
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -4747,6 +5421,7 @@
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -4822,6 +5497,7 @@
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4897,6 +5573,7 @@
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4972,6 +5649,7 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -5047,6 +5725,7 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -5122,6 +5801,7 @@
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -5197,6 +5877,7 @@
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -5272,6 +5953,7 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -5347,6 +6029,7 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -5422,6 +6105,7 @@
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -5497,6 +6181,7 @@
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -5572,6 +6257,7 @@
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -5647,6 +6333,7 @@
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -5722,6 +6409,7 @@
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -5797,6 +6485,7 @@
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -5872,6 +6561,7 @@
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -5947,6 +6637,7 @@
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -6022,6 +6713,7 @@
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -6097,6 +6789,7 @@
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -6172,6 +6865,7 @@
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -6247,6 +6941,7 @@
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -6322,6 +7017,7 @@
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -6397,6 +7093,7 @@
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -6472,6 +7169,7 @@
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -6547,6 +7245,7 @@
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -6622,6 +7321,7 @@
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -6697,6 +7397,7 @@
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -6772,6 +7473,7 @@
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -6847,6 +7549,7 @@
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -6909,7 +7612,7 @@
       <c r="BP62" s="9"/>
       <c r="BQ62" s="9"/>
     </row>
-    <row r="63" spans="1:69" ht="16.5" thickBot="1">
+    <row r="63" spans="1:69" ht="32.25" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>126</v>
       </c>
@@ -6922,6 +7625,7 @@
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -6997,6 +7701,7 @@
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -7072,6 +7777,7 @@
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -7147,6 +7853,7 @@
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -7222,6 +7929,7 @@
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -7297,6 +8005,7 @@
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -7372,6 +8081,7 @@
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -7447,6 +8157,7 @@
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -7509,7 +8220,7 @@
       <c r="BP70" s="9"/>
       <c r="BQ70" s="9"/>
     </row>
-    <row r="71" spans="1:69" ht="16.5" thickBot="1">
+    <row r="71" spans="1:69" ht="32.25" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>143</v>
       </c>
@@ -7522,6 +8233,7 @@
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -7597,6 +8309,7 @@
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -7672,6 +8385,7 @@
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -7747,6 +8461,7 @@
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -7822,6 +8537,7 @@
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -7897,6 +8613,7 @@
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
@@ -7972,6 +8689,7 @@
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
@@ -8047,6 +8765,7 @@
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -8122,6 +8841,7 @@
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -8197,6 +8917,7 @@
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -8272,6 +8993,7 @@
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -8347,6 +9069,7 @@
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -8422,6 +9145,7 @@
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
@@ -8497,6 +9221,7 @@
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
@@ -8572,6 +9297,7 @@
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
@@ -8647,6 +9373,7 @@
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
@@ -8722,6 +9449,7 @@
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
@@ -8797,6 +9525,7 @@
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
@@ -8872,6 +9601,7 @@
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -8947,6 +9677,7 @@
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
@@ -9022,6 +9753,7 @@
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -9097,6 +9829,7 @@
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -9172,6 +9905,7 @@
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -9247,6 +9981,7 @@
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -9322,6 +10057,7 @@
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
       <c r="I95" s="9"/>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -9397,6 +10133,7 @@
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -9472,6 +10209,7 @@
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -9547,6 +10285,7 @@
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -9622,6 +10361,7 @@
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
       <c r="I99" s="9"/>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -9697,6 +10437,7 @@
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
       <c r="I100" s="9"/>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -9772,6 +10513,7 @@
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -9847,6 +10589,7 @@
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -9922,6 +10665,7 @@
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
       <c r="I103" s="9"/>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -9997,6 +10741,7 @@
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -10072,6 +10817,7 @@
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
       <c r="I105" s="9"/>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -10147,6 +10893,7 @@
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
       <c r="I106" s="9"/>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -10222,6 +10969,7 @@
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
       <c r="I107" s="9"/>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -10297,6 +11045,7 @@
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
       <c r="I108" s="9"/>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -10372,6 +11121,7 @@
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
       <c r="I109" s="9"/>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -10447,6 +11197,7 @@
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
       <c r="I110" s="9"/>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -10522,6 +11273,7 @@
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
       <c r="I111" s="9"/>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -10597,6 +11349,7 @@
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
       <c r="I112" s="9"/>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -10672,6 +11425,7 @@
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
       <c r="I113" s="9"/>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
@@ -10747,6 +11501,7 @@
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
       <c r="I114" s="9"/>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
@@ -10822,6 +11577,7 @@
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
       <c r="I115" s="9"/>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
@@ -10897,6 +11653,7 @@
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
       <c r="I116" s="9"/>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
@@ -10972,6 +11729,7 @@
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
       <c r="I117" s="9"/>
       <c r="J117" s="9"/>
       <c r="K117" s="9"/>
@@ -11047,6 +11805,7 @@
       </c>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
       <c r="I118" s="9"/>
       <c r="J118" s="9"/>
       <c r="K118" s="9"/>
@@ -11122,6 +11881,7 @@
       </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
       <c r="I119" s="9"/>
       <c r="J119" s="9"/>
       <c r="K119" s="9"/>
@@ -11197,6 +11957,7 @@
       </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
       <c r="I120" s="9"/>
       <c r="J120" s="9"/>
       <c r="K120" s="9"/>
@@ -11272,6 +12033,7 @@
       </c>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
       <c r="I121" s="9"/>
       <c r="J121" s="9"/>
       <c r="K121" s="9"/>
@@ -11347,6 +12109,7 @@
       </c>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
       <c r="I122" s="9"/>
       <c r="J122" s="9"/>
       <c r="K122" s="9"/>
@@ -11422,6 +12185,7 @@
       </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
       <c r="I123" s="9"/>
       <c r="J123" s="9"/>
       <c r="K123" s="9"/>
@@ -11497,6 +12261,7 @@
       </c>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
       <c r="I124" s="9"/>
       <c r="J124" s="9"/>
       <c r="K124" s="9"/>
@@ -11572,6 +12337,7 @@
       </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
       <c r="I125" s="9"/>
       <c r="J125" s="9"/>
       <c r="K125" s="9"/>
@@ -11647,6 +12413,7 @@
       </c>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
       <c r="I126" s="9"/>
       <c r="J126" s="9"/>
       <c r="K126" s="9"/>
@@ -11722,6 +12489,7 @@
       </c>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
       <c r="I127" s="9"/>
       <c r="J127" s="9"/>
       <c r="K127" s="9"/>
@@ -11797,6 +12565,7 @@
       </c>
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
       <c r="I128" s="9"/>
       <c r="J128" s="9"/>
       <c r="K128" s="9"/>
@@ -11859,7 +12628,7 @@
       <c r="BP128" s="9"/>
       <c r="BQ128" s="9"/>
     </row>
-    <row r="129" spans="1:69" ht="16.5" thickBot="1">
+    <row r="129" spans="1:69" ht="32.25" thickBot="1">
       <c r="A129" s="3" t="s">
         <v>260</v>
       </c>
@@ -11872,6 +12641,7 @@
       </c>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
       <c r="I129" s="9"/>
       <c r="J129" s="9"/>
       <c r="K129" s="9"/>
@@ -11947,6 +12717,7 @@
       </c>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
       <c r="I130" s="9"/>
       <c r="J130" s="9"/>
       <c r="K130" s="9"/>
@@ -12022,6 +12793,7 @@
       </c>
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
       <c r="I131" s="9"/>
       <c r="J131" s="9"/>
       <c r="K131" s="9"/>
@@ -12097,6 +12869,7 @@
       </c>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
       <c r="I132" s="9"/>
       <c r="J132" s="9"/>
       <c r="K132" s="9"/>
@@ -12172,6 +12945,7 @@
       </c>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
       <c r="I133" s="9"/>
       <c r="J133" s="9"/>
       <c r="K133" s="9"/>
@@ -12247,6 +13021,7 @@
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
       <c r="I134" s="9"/>
       <c r="J134" s="9"/>
       <c r="K134" s="9"/>
@@ -12322,6 +13097,7 @@
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
       <c r="I135" s="9"/>
       <c r="J135" s="9"/>
       <c r="K135" s="9"/>
@@ -12397,6 +13173,7 @@
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
       <c r="I136" s="9"/>
       <c r="J136" s="9"/>
       <c r="K136" s="9"/>
@@ -12472,6 +13249,7 @@
       </c>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
       <c r="I137" s="9"/>
       <c r="J137" s="9"/>
       <c r="K137" s="9"/>
@@ -12547,6 +13325,7 @@
       </c>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
       <c r="K138" s="9"/>
@@ -12622,6 +13401,7 @@
       </c>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
       <c r="I139" s="9"/>
       <c r="J139" s="9"/>
       <c r="K139" s="9"/>
@@ -12697,6 +13477,7 @@
       </c>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
       <c r="I140" s="9"/>
       <c r="J140" s="9"/>
       <c r="K140" s="9"/>
@@ -12772,6 +13553,7 @@
       </c>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
       <c r="K141" s="9"/>
@@ -12847,6 +13629,7 @@
       </c>
       <c r="E142" s="4"/>
       <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
       <c r="K142" s="9"/>
@@ -12922,6 +13705,7 @@
       </c>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
       <c r="I143" s="9"/>
       <c r="J143" s="9"/>
       <c r="K143" s="9"/>
@@ -12997,6 +13781,7 @@
       </c>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
       <c r="K144" s="9"/>
@@ -13072,6 +13857,7 @@
       </c>
       <c r="E145" s="4"/>
       <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
       <c r="I145" s="9"/>
       <c r="J145" s="9"/>
       <c r="K145" s="9"/>
@@ -13147,6 +13933,7 @@
       </c>
       <c r="E146" s="4"/>
       <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
       <c r="I146" s="9"/>
       <c r="J146" s="9"/>
       <c r="K146" s="9"/>
@@ -13222,6 +14009,7 @@
       </c>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
       <c r="I147" s="9"/>
       <c r="J147" s="9"/>
       <c r="K147" s="9"/>
@@ -13297,6 +14085,7 @@
       </c>
       <c r="E148" s="4"/>
       <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
       <c r="I148" s="9"/>
       <c r="J148" s="9"/>
       <c r="K148" s="9"/>
@@ -13372,6 +14161,7 @@
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
       <c r="K149" s="9"/>
@@ -13447,6 +14237,7 @@
       </c>
       <c r="E150" s="4"/>
       <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
       <c r="I150" s="9"/>
       <c r="J150" s="9"/>
       <c r="K150" s="9"/>
@@ -13522,6 +14313,7 @@
       </c>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
       <c r="I151" s="9"/>
       <c r="J151" s="9"/>
       <c r="K151" s="9"/>
@@ -13597,6 +14389,7 @@
       </c>
       <c r="E152" s="4"/>
       <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
       <c r="I152" s="9"/>
       <c r="J152" s="9"/>
       <c r="K152" s="9"/>
@@ -13672,6 +14465,7 @@
       </c>
       <c r="E153" s="4"/>
       <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
       <c r="I153" s="9"/>
       <c r="J153" s="9"/>
       <c r="K153" s="9"/>
@@ -13747,6 +14541,7 @@
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
       <c r="I154" s="9"/>
       <c r="J154" s="9"/>
       <c r="K154" s="9"/>
@@ -13822,6 +14617,7 @@
       </c>
       <c r="E155" s="4"/>
       <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
       <c r="I155" s="9"/>
       <c r="J155" s="9"/>
       <c r="K155" s="9"/>
@@ -13897,6 +14693,7 @@
       </c>
       <c r="E156" s="4"/>
       <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
       <c r="I156" s="9"/>
       <c r="J156" s="9"/>
       <c r="K156" s="9"/>
@@ -13972,6 +14769,7 @@
       </c>
       <c r="E157" s="4"/>
       <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
       <c r="K157" s="9"/>
@@ -14047,6 +14845,7 @@
       </c>
       <c r="E158" s="4"/>
       <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
       <c r="I158" s="9"/>
       <c r="J158" s="9"/>
       <c r="K158" s="9"/>
@@ -14122,6 +14921,7 @@
       </c>
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
       <c r="I159" s="9"/>
       <c r="J159" s="9"/>
       <c r="K159" s="9"/>
@@ -14197,6 +14997,7 @@
       </c>
       <c r="E160" s="4"/>
       <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
       <c r="I160" s="9"/>
       <c r="J160" s="9"/>
       <c r="K160" s="9"/>
@@ -14272,6 +15073,7 @@
       </c>
       <c r="E161" s="4"/>
       <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
       <c r="K161" s="9"/>
@@ -14347,6 +15149,7 @@
       </c>
       <c r="E162" s="4"/>
       <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
       <c r="I162" s="9"/>
       <c r="J162" s="9"/>
       <c r="K162" s="9"/>
@@ -14422,6 +15225,7 @@
       </c>
       <c r="E163" s="4"/>
       <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
       <c r="I163" s="9"/>
       <c r="J163" s="9"/>
       <c r="K163" s="9"/>
@@ -14497,6 +15301,7 @@
       </c>
       <c r="E164" s="4"/>
       <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
       <c r="I164" s="9"/>
       <c r="J164" s="9"/>
       <c r="K164" s="9"/>
@@ -14572,6 +15377,7 @@
       </c>
       <c r="E165" s="4"/>
       <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
       <c r="I165" s="9"/>
       <c r="J165" s="9"/>
       <c r="K165" s="9"/>
@@ -14647,6 +15453,7 @@
       </c>
       <c r="E166" s="4"/>
       <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
       <c r="I166" s="9"/>
       <c r="J166" s="9"/>
       <c r="K166" s="9"/>
@@ -14722,6 +15529,7 @@
       </c>
       <c r="E167" s="4"/>
       <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
       <c r="I167" s="9"/>
       <c r="J167" s="9"/>
       <c r="K167" s="9"/>
@@ -14797,6 +15605,7 @@
       </c>
       <c r="E168" s="4"/>
       <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
       <c r="I168" s="9"/>
       <c r="J168" s="9"/>
       <c r="K168" s="9"/>
@@ -14872,6 +15681,7 @@
       </c>
       <c r="E169" s="4"/>
       <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
       <c r="I169" s="9"/>
       <c r="J169" s="9"/>
       <c r="K169" s="9"/>
@@ -14947,6 +15757,7 @@
       </c>
       <c r="E170" s="4"/>
       <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
       <c r="I170" s="9"/>
       <c r="J170" s="9"/>
       <c r="K170" s="9"/>
@@ -15022,6 +15833,7 @@
       </c>
       <c r="E171" s="4"/>
       <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
       <c r="I171" s="9"/>
       <c r="J171" s="9"/>
       <c r="K171" s="9"/>
@@ -15097,6 +15909,7 @@
       </c>
       <c r="E172" s="4"/>
       <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
       <c r="I172" s="9"/>
       <c r="J172" s="9"/>
       <c r="K172" s="9"/>
@@ -15172,6 +15985,7 @@
       </c>
       <c r="E173" s="4"/>
       <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
       <c r="I173" s="9"/>
       <c r="J173" s="9"/>
       <c r="K173" s="9"/>
@@ -15247,6 +16061,7 @@
       </c>
       <c r="E174" s="4"/>
       <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
       <c r="I174" s="9"/>
       <c r="J174" s="9"/>
       <c r="K174" s="9"/>
@@ -15322,6 +16137,7 @@
       </c>
       <c r="E175" s="4"/>
       <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
       <c r="I175" s="9"/>
       <c r="J175" s="9"/>
       <c r="K175" s="9"/>
@@ -15397,6 +16213,7 @@
       </c>
       <c r="E176" s="4"/>
       <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
       <c r="I176" s="9"/>
       <c r="J176" s="9"/>
       <c r="K176" s="9"/>
@@ -15472,6 +16289,7 @@
       </c>
       <c r="E177" s="4"/>
       <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
       <c r="I177" s="9"/>
       <c r="J177" s="9"/>
       <c r="K177" s="9"/>
@@ -15547,6 +16365,7 @@
       </c>
       <c r="E178" s="4"/>
       <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
       <c r="I178" s="9"/>
       <c r="J178" s="9"/>
       <c r="K178" s="9"/>
@@ -15622,6 +16441,7 @@
       </c>
       <c r="E179" s="4"/>
       <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
       <c r="I179" s="9"/>
       <c r="J179" s="9"/>
       <c r="K179" s="9"/>
@@ -15697,6 +16517,7 @@
       </c>
       <c r="E180" s="4"/>
       <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
       <c r="I180" s="9"/>
       <c r="J180" s="9"/>
       <c r="K180" s="9"/>
@@ -15759,7 +16580,7 @@
       <c r="BP180" s="9"/>
       <c r="BQ180" s="9"/>
     </row>
-    <row r="181" spans="1:69" ht="16.5" thickBot="1">
+    <row r="181" spans="1:69" ht="32.25" thickBot="1">
       <c r="A181" s="3" t="s">
         <v>367</v>
       </c>
@@ -15772,6 +16593,7 @@
       </c>
       <c r="E181" s="4"/>
       <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
       <c r="I181" s="9"/>
       <c r="J181" s="9"/>
       <c r="K181" s="9"/>
@@ -15847,6 +16669,7 @@
       </c>
       <c r="E182" s="4"/>
       <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
       <c r="I182" s="9"/>
       <c r="J182" s="9"/>
       <c r="K182" s="9"/>
@@ -15922,6 +16745,7 @@
       </c>
       <c r="E183" s="4"/>
       <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
       <c r="I183" s="9"/>
       <c r="J183" s="9"/>
       <c r="K183" s="9"/>
@@ -15997,6 +16821,7 @@
       </c>
       <c r="E184" s="4"/>
       <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
       <c r="I184" s="9"/>
       <c r="J184" s="9"/>
       <c r="K184" s="9"/>
@@ -16072,6 +16897,7 @@
       </c>
       <c r="E185" s="4"/>
       <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
       <c r="I185" s="9"/>
       <c r="J185" s="9"/>
       <c r="K185" s="9"/>
@@ -16147,6 +16973,7 @@
       </c>
       <c r="E186" s="4"/>
       <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
       <c r="I186" s="9"/>
       <c r="J186" s="9"/>
       <c r="K186" s="9"/>
@@ -16209,7 +17036,7 @@
       <c r="BP186" s="9"/>
       <c r="BQ186" s="9"/>
     </row>
-    <row r="187" spans="1:69" ht="16.5" thickBot="1">
+    <row r="187" spans="1:69" ht="32.25" thickBot="1">
       <c r="A187" s="3" t="s">
         <v>379</v>
       </c>
@@ -16222,6 +17049,7 @@
       </c>
       <c r="E187" s="4"/>
       <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
       <c r="I187" s="9"/>
       <c r="J187" s="9"/>
       <c r="K187" s="9"/>
@@ -16284,7 +17112,7 @@
       <c r="BP187" s="9"/>
       <c r="BQ187" s="9"/>
     </row>
-    <row r="188" spans="1:69" ht="16.5" thickBot="1">
+    <row r="188" spans="1:69" ht="32.25" thickBot="1">
       <c r="A188" s="3" t="s">
         <v>381</v>
       </c>
@@ -16297,6 +17125,7 @@
       </c>
       <c r="E188" s="4"/>
       <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
       <c r="I188" s="9"/>
       <c r="J188" s="9"/>
       <c r="K188" s="9"/>
@@ -16372,6 +17201,7 @@
       </c>
       <c r="E189" s="4"/>
       <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
       <c r="I189" s="9"/>
       <c r="J189" s="9"/>
       <c r="K189" s="9"/>
@@ -16447,6 +17277,7 @@
       </c>
       <c r="E190" s="4"/>
       <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
       <c r="I190" s="9"/>
       <c r="J190" s="9"/>
       <c r="K190" s="9"/>
@@ -16522,6 +17353,7 @@
       </c>
       <c r="E191" s="4"/>
       <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
       <c r="I191" s="9"/>
       <c r="J191" s="9"/>
       <c r="K191" s="9"/>
@@ -16597,6 +17429,7 @@
       </c>
       <c r="E192" s="4"/>
       <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
       <c r="I192" s="9"/>
       <c r="J192" s="9"/>
       <c r="K192" s="9"/>
@@ -16672,6 +17505,7 @@
       </c>
       <c r="E193" s="4"/>
       <c r="F193" s="4"/>
+      <c r="G193" s="4"/>
       <c r="I193" s="9"/>
       <c r="J193" s="9"/>
       <c r="K193" s="9"/>
@@ -16747,6 +17581,7 @@
       </c>
       <c r="E194" s="4"/>
       <c r="F194" s="4"/>
+      <c r="G194" s="4"/>
       <c r="I194" s="9"/>
       <c r="J194" s="9"/>
       <c r="K194" s="9"/>
@@ -16822,6 +17657,7 @@
       </c>
       <c r="E195" s="4"/>
       <c r="F195" s="4"/>
+      <c r="G195" s="4"/>
       <c r="I195" s="9"/>
       <c r="J195" s="9"/>
       <c r="K195" s="9"/>
@@ -16897,6 +17733,7 @@
       </c>
       <c r="E196" s="4"/>
       <c r="F196" s="4"/>
+      <c r="G196" s="4"/>
       <c r="I196" s="9"/>
       <c r="J196" s="9"/>
       <c r="K196" s="9"/>
@@ -16972,6 +17809,7 @@
       </c>
       <c r="E197" s="4"/>
       <c r="F197" s="4"/>
+      <c r="G197" s="4"/>
       <c r="I197" s="9"/>
       <c r="J197" s="9"/>
       <c r="K197" s="9"/>
@@ -17047,6 +17885,7 @@
       </c>
       <c r="E198" s="4"/>
       <c r="F198" s="4"/>
+      <c r="G198" s="4"/>
       <c r="I198" s="9"/>
       <c r="J198" s="9"/>
       <c r="K198" s="9"/>
@@ -17122,6 +17961,7 @@
       </c>
       <c r="E199" s="4"/>
       <c r="F199" s="4"/>
+      <c r="G199" s="4"/>
       <c r="I199" s="9"/>
       <c r="J199" s="9"/>
       <c r="K199" s="9"/>
@@ -17197,6 +18037,7 @@
       </c>
       <c r="E200" s="4"/>
       <c r="F200" s="4"/>
+      <c r="G200" s="4"/>
       <c r="I200" s="9"/>
       <c r="J200" s="9"/>
       <c r="K200" s="9"/>
@@ -17272,6 +18113,7 @@
       </c>
       <c r="E201" s="4"/>
       <c r="F201" s="4"/>
+      <c r="G201" s="4"/>
       <c r="I201" s="9"/>
       <c r="J201" s="9"/>
       <c r="K201" s="9"/>
@@ -17347,6 +18189,7 @@
       </c>
       <c r="E202" s="4"/>
       <c r="F202" s="4"/>
+      <c r="G202" s="4"/>
       <c r="I202" s="9"/>
       <c r="J202" s="9"/>
       <c r="K202" s="9"/>
@@ -17409,7 +18252,7 @@
       <c r="BP202" s="9"/>
       <c r="BQ202" s="9"/>
     </row>
-    <row r="203" spans="1:69" ht="16.5" thickBot="1">
+    <row r="203" spans="1:69" ht="32.25" thickBot="1">
       <c r="A203" s="3" t="s">
         <v>412</v>
       </c>
@@ -17422,6 +18265,7 @@
       </c>
       <c r="E203" s="4"/>
       <c r="F203" s="4"/>
+      <c r="G203" s="4"/>
       <c r="I203" s="9"/>
       <c r="J203" s="9"/>
       <c r="K203" s="9"/>
@@ -17497,6 +18341,7 @@
       </c>
       <c r="E204" s="4"/>
       <c r="F204" s="4"/>
+      <c r="G204" s="4"/>
       <c r="I204" s="9"/>
       <c r="J204" s="9"/>
       <c r="K204" s="9"/>
@@ -17572,6 +18417,7 @@
       </c>
       <c r="E205" s="4"/>
       <c r="F205" s="4"/>
+      <c r="G205" s="4"/>
       <c r="I205" s="9"/>
       <c r="J205" s="9"/>
       <c r="K205" s="9"/>
@@ -17647,6 +18493,7 @@
       </c>
       <c r="E206" s="4"/>
       <c r="F206" s="4"/>
+      <c r="G206" s="4"/>
       <c r="I206" s="9"/>
       <c r="J206" s="9"/>
       <c r="K206" s="9"/>
@@ -17722,6 +18569,7 @@
       </c>
       <c r="E207" s="4"/>
       <c r="F207" s="4"/>
+      <c r="G207" s="4"/>
       <c r="I207" s="9"/>
       <c r="J207" s="9"/>
       <c r="K207" s="9"/>
@@ -17797,6 +18645,7 @@
       </c>
       <c r="E208" s="4"/>
       <c r="F208" s="4"/>
+      <c r="G208" s="4"/>
       <c r="I208" s="9"/>
       <c r="J208" s="9"/>
       <c r="K208" s="9"/>
@@ -17872,6 +18721,7 @@
       </c>
       <c r="E209" s="4"/>
       <c r="F209" s="4"/>
+      <c r="G209" s="4"/>
       <c r="I209" s="9"/>
       <c r="J209" s="9"/>
       <c r="K209" s="9"/>
@@ -17947,6 +18797,7 @@
       </c>
       <c r="E210" s="4"/>
       <c r="F210" s="4"/>
+      <c r="G210" s="4"/>
       <c r="I210" s="9"/>
       <c r="J210" s="9"/>
       <c r="K210" s="9"/>
@@ -18022,6 +18873,7 @@
       </c>
       <c r="E211" s="4"/>
       <c r="F211" s="4"/>
+      <c r="G211" s="4"/>
       <c r="I211" s="9"/>
       <c r="J211" s="9"/>
       <c r="K211" s="9"/>
@@ -18084,7 +18936,7 @@
       <c r="BP211" s="9"/>
       <c r="BQ211" s="9"/>
     </row>
-    <row r="212" spans="1:69" ht="16.5" thickBot="1">
+    <row r="212" spans="1:69" ht="32.25" thickBot="1">
       <c r="A212" s="3" t="s">
         <v>430</v>
       </c>
@@ -18097,6 +18949,7 @@
       </c>
       <c r="E212" s="4"/>
       <c r="F212" s="4"/>
+      <c r="G212" s="4"/>
       <c r="I212" s="9"/>
       <c r="J212" s="9"/>
       <c r="K212" s="9"/>
@@ -18172,6 +19025,7 @@
       </c>
       <c r="E213" s="4"/>
       <c r="F213" s="4"/>
+      <c r="G213" s="4"/>
       <c r="I213" s="9"/>
       <c r="J213" s="9"/>
       <c r="K213" s="9"/>
@@ -18247,6 +19101,7 @@
       </c>
       <c r="E214" s="4"/>
       <c r="F214" s="4"/>
+      <c r="G214" s="4"/>
       <c r="I214" s="9"/>
       <c r="J214" s="9"/>
       <c r="K214" s="9"/>
@@ -18322,6 +19177,7 @@
       </c>
       <c r="E215" s="4"/>
       <c r="F215" s="4"/>
+      <c r="G215" s="4"/>
       <c r="I215" s="9"/>
       <c r="J215" s="9"/>
       <c r="K215" s="9"/>
@@ -18384,7 +19240,7 @@
       <c r="BP215" s="9"/>
       <c r="BQ215" s="9"/>
     </row>
-    <row r="216" spans="1:69" ht="201.75">
+    <row r="216" spans="1:69" ht="200.25">
       <c r="I216" s="6" t="s">
         <v>485</v>
       </c>
@@ -18549,11 +19405,11 @@
       </c>
       <c r="I217">
         <f>SUM(I3:I215)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J217">
         <f t="shared" ref="J217:BQ217" si="0">SUM(J3:J215)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K217">
         <f t="shared" si="0"/>
@@ -18561,15 +19417,15 @@
       </c>
       <c r="L217">
         <f>SUM(L3:L215)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P217">
         <f t="shared" si="0"/>
@@ -18577,67 +19433,67 @@
       </c>
       <c r="Q217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S217">
         <f>SUM(S3:S215)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AJ217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK217">
         <f t="shared" si="0"/>
@@ -18645,7 +19501,7 @@
       </c>
       <c r="AL217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM217">
         <f t="shared" si="0"/>
@@ -18653,7 +19509,7 @@
       </c>
       <c r="AO217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AP217">
         <f t="shared" si="0"/>
@@ -18669,7 +19525,7 @@
       </c>
       <c r="AS217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT217">
         <f t="shared" si="0"/>
@@ -18677,27 +19533,27 @@
       </c>
       <c r="AU217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW217">
         <f>SUM(AW3:AW215)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AY217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ217">
         <f>SUM(AZ3:AZ215)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BB217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BD217" s="12">
         <f t="shared" si="0"/>
@@ -18705,34 +19561,34 @@
       </c>
       <c r="BE217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BF217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG217" s="12" t="s">
         <v>482</v>
       </c>
       <c r="BH217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BI217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BK217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BL217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BN217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO217">
         <f t="shared" si="0"/>
@@ -18757,24 +19613,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task 12 - Zaktualizaować rozdział 1
</commit_message>
<xml_diff>
--- a/dane_aplikacji.xlsx
+++ b/dane_aplikacji.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="582">
   <si>
     <t>Id</t>
   </si>
@@ -1776,6 +1776,12 @@
   </si>
   <si>
     <t>18-11-2014</t>
+  </si>
+  <si>
+    <t>stosuje się do zalecień</t>
+  </si>
+  <si>
+    <t>nie stosuje się do zalecień</t>
   </si>
 </sst>
 </file>
@@ -2168,14 +2174,13 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="79535488"/>
-        <c:axId val="79557760"/>
+        <c:axId val="59605760"/>
+        <c:axId val="59607296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79535488"/>
+        <c:axId val="59605760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2216,14 +2221,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79557760"/>
+        <c:crossAx val="59607296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79557760"/>
+        <c:axId val="59607296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79535488"/>
+        <c:crossAx val="59605760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2312,6 +2317,1066 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AY$215:$AZ$215</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>umozliwia udostępnianie </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brak udostepnainia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AY$216:$AZ$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BB$215:$BC$215</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>używany splashscreen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brak splashscreen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BB$216:$BC$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BE$215:$BF$215</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>posiada ustawienia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bez ustawień</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BE$216:$BF$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BH$215:$BI$215</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>stosuje się do zalecień</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nie stosuje się do zalecień</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BH$216:$BI$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$215:$L$215</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>okna pop-up</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>toast</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>powiadomienia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>komunikaty osadzone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$216:$L$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="90949888"/>
+        <c:axId val="92536832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90949888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92536832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92536832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90949888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$215:$S$215</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>logowanie klasyczne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brak logowania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>logowanie automatyczne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>logowanie przez FB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>logowanie przez G+</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>logowanie opcjonalneopcjonalne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$216:$S$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="112145536"/>
+        <c:axId val="112147072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="112145536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112147072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112147072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112145536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$U$215:$X$215</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>zawieszanie się aplikacji</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brak widocznego ładowania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ładowanie z paskiem postepu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ładowanie bez bez paska postępu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$216:$X$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="113985024"/>
+        <c:axId val="114001408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113985024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114001408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="114001408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113985024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$Z$215:$AE$215</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v> menu lista</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>menu kafelki</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>menu wysówane z lewej krawedzi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>menu wysówane z przycisku</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>menu natywne</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>menu Action Bar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$216:$AE$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="113938432"/>
+        <c:axId val="113940736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113938432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113940736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="113940736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113938432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1932952689376644E-2"/>
+                  <c:y val="6.8701063003543186E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.9010954838527468E-2"/>
+                  <c:y val="-1.472825553146561E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AG$215:$AH$215</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>informuje o nawigacji</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brak jakiejkowliek informacji</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AG$216:$AH$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$215:$AM$215</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>brak reklam</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>reklamuy w powiadomieniach</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>reklamy banerowe</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>reklamy pełnoekranowe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$216:$AM$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="114321664"/>
+        <c:axId val="114420736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="114321664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114420736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="114420736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114321664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AO$215:$AQ$215</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>poprawne wg materiałów treningowych</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pokrywa treść</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>elementy klikalne zbyt blisko</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AO$216:$AQ$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:axId val="112175744"/>
+        <c:axId val="112233088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="112175744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112233088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112233088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112175744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14929954917550878"/>
+                  <c:y val="-0.20463254818717261"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AS$215:$AW$215</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>rejestracja klasyczna</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>rejestracja wieloetapowa</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>rejestracja przez web</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rejestracja automatycznaauto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>brak rejestracji</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AS$216:$AW$216</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>141</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2896,6 +3961,371 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>911679</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>911678</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>911679</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>925284</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>925285</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>911679</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>925285</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>911679</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>898070</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>898072</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>900545</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>103909</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>935181</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121226</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3181,10 +4611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ217"/>
+  <dimension ref="A1:BQ223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C194" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BS210" sqref="BS210"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G224" sqref="G224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3210,14 +4640,16 @@
     <col min="30" max="31" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="0.7109375" style="12" customWidth="1"/>
     <col min="33" max="33" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="0.85546875" style="12" customWidth="1"/>
-    <col min="36" max="39" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="4" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="1.140625" style="12" customWidth="1"/>
     <col min="41" max="42" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="1.140625" style="12" customWidth="1"/>
-    <col min="45" max="49" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="48" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="1" style="12" customWidth="1"/>
     <col min="51" max="51" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="5" bestFit="1" customWidth="1"/>
@@ -3228,10 +4660,10 @@
     <col min="57" max="57" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="1" style="12" customWidth="1"/>
-    <col min="60" max="60" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="1" style="12" customWidth="1"/>
-    <col min="63" max="63" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="1.140625" style="12" customWidth="1"/>
     <col min="66" max="69" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -26967,7 +28399,7 @@
       <c r="BP214" s="48"/>
       <c r="BQ214" s="48"/>
     </row>
-    <row r="215" spans="1:69" ht="201.75">
+    <row r="215" spans="1:69" ht="204">
       <c r="D215" s="24"/>
       <c r="I215" s="6" t="s">
         <v>482</v>
@@ -27103,10 +28535,10 @@
         <v>479</v>
       </c>
       <c r="BH215" s="6" t="s">
-        <v>475</v>
+        <v>580</v>
       </c>
       <c r="BI215" s="6" t="s">
-        <v>476</v>
+        <v>581</v>
       </c>
       <c r="BK215" s="6" t="s">
         <v>520</v>
@@ -27216,12 +28648,12 @@
         <v>43</v>
       </c>
       <c r="AH216">
-        <f t="shared" si="0"/>
-        <v>145</v>
+        <f>210-AG216</f>
+        <v>167</v>
       </c>
       <c r="AJ216">
-        <f t="shared" si="0"/>
-        <v>114</v>
+        <f>210-AL216</f>
+        <v>140</v>
       </c>
       <c r="AK216">
         <f t="shared" si="0"/>
@@ -27268,24 +28700,24 @@
         <v>23</v>
       </c>
       <c r="AW216">
-        <f>SUM(AW3:AW214)</f>
-        <v>131</v>
+        <f>210-AS216-AT216-AU216-AV216</f>
+        <v>141</v>
       </c>
       <c r="AY216">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="AZ216">
-        <f>SUM(AZ3:AZ214)</f>
-        <v>136</v>
+        <f>210-AY216</f>
+        <v>152</v>
       </c>
       <c r="BB216">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="BC216">
-        <f t="shared" si="0"/>
-        <v>125</v>
+        <f>210-BB216</f>
+        <v>139</v>
       </c>
       <c r="BD216" s="12">
         <f t="shared" si="0"/>
@@ -27296,23 +28728,23 @@
         <v>128</v>
       </c>
       <c r="BF216">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f>210-BE216</f>
+        <v>82</v>
       </c>
       <c r="BG216" s="12" t="s">
         <v>479</v>
       </c>
       <c r="BH216">
-        <f t="shared" si="0"/>
-        <v>167</v>
+        <f>210-BI216</f>
+        <v>183</v>
       </c>
       <c r="BI216">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="BK216">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>210-BL216</f>
+        <v>201</v>
       </c>
       <c r="BL216">
         <f t="shared" si="0"/>
@@ -27338,9 +28770,16 @@
     <row r="217" spans="1:69" ht="15.75">
       <c r="A217" s="5"/>
     </row>
+    <row r="223" spans="1:69">
+      <c r="G223">
+        <f>183/210</f>
+        <v>0.87142857142857144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>